<commit_message>
Stores itemtype and property values in dictionary the sends this to query method and erases dictionary for next itemtype/its properties
</commit_message>
<xml_diff>
--- a/Width Lengths.xlsx
+++ b/Width Lengths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyGit\SQLQueryCreator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F93AC8-86AD-4E95-BE0A-9E4E3B2C5A75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469D6E3C-5985-4F89-B237-DB5440DEB5DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53835" yWindow="3195" windowWidth="19995" windowHeight="12315" xr2:uid="{BCF4C9D9-7C86-41C2-945B-B1551F976C53}"/>
+    <workbookView xWindow="7" yWindow="0" windowWidth="19993" windowHeight="12313" xr2:uid="{BCF4C9D9-7C86-41C2-945B-B1551F976C53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="404">
   <si>
     <t>ItemType</t>
   </si>
@@ -1606,10 +1606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B85F58-F77E-477C-B8F3-CE1AD8EBE719}">
-  <dimension ref="A1:BL792"/>
+  <dimension ref="A1:BL793"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1736,6 +1736,9 @@
     </row>
     <row r="6" spans="1:64" x14ac:dyDescent="0.5">
       <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="H6" t="s">
         <v>9</v>
       </c>
@@ -1798,7 +1801,9 @@
     </row>
     <row r="14" spans="1:64" x14ac:dyDescent="0.5">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:64" x14ac:dyDescent="0.5">
@@ -1863,6 +1868,12 @@
       </c>
       <c r="E19">
         <v>992</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.5">
@@ -1875,7 +1886,9 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="B21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A22" s="1"/>
@@ -1923,7 +1936,9 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="B29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
@@ -1948,7 +1963,9 @@
       </c>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.5">
-      <c r="B35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.5">
       <c r="A36" s="1"/>
@@ -2045,6 +2062,9 @@
       <c r="E43">
         <v>519</v>
       </c>
+      <c r="H43" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="N43" t="s">
         <v>360</v>
       </c>
@@ -2117,6 +2137,12 @@
       </c>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.5">
+      <c r="B46" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="T46" t="s">
         <v>367</v>
       </c>
@@ -2131,6 +2157,9 @@
       </c>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.5">
+      <c r="T47" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="AA47" t="s">
         <v>373</v>
       </c>
@@ -2140,6 +2169,9 @@
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.5">
       <c r="B48" s="1"/>
+      <c r="AA48" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.5">
       <c r="B49" s="1"/>
@@ -2182,6 +2214,9 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B53" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="H53" t="s">
         <v>3</v>
       </c>
@@ -2199,6 +2234,9 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.5">
       <c r="B55" s="1"/>
+      <c r="H55" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.5">
       <c r="B56" s="1"/>
@@ -2239,7 +2277,9 @@
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="B62" s="1"/>
+      <c r="B62" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.5">
       <c r="B63" s="1"/>
@@ -2264,7 +2304,9 @@
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="B67" s="1"/>
+      <c r="B67" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.5">
       <c r="B68" s="1"/>
@@ -2313,7 +2355,9 @@
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="B75" s="1"/>
+      <c r="B75" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A78" s="1" t="s">
@@ -2398,6 +2442,9 @@
       <c r="E84">
         <v>141</v>
       </c>
+      <c r="H84" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B85" t="s">
@@ -2415,6 +2462,11 @@
         <v>80</v>
       </c>
     </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B87" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A89" s="1" t="s">
         <v>0</v>
@@ -2517,6 +2569,17 @@
       <c r="K94">
         <v>635</v>
       </c>
+      <c r="N94" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B95" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A98" s="1" t="s">
@@ -2581,6 +2644,9 @@
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B103" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="H103" t="s">
         <v>59</v>
       </c>
@@ -2596,6 +2662,11 @@
         <v>441</v>
       </c>
     </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="H105" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A107" s="1" t="s">
         <v>0</v>
@@ -2613,6 +2684,11 @@
       </c>
       <c r="E109">
         <v>399</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B110" s="1" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.5">
@@ -2642,6 +2718,11 @@
         <v>963</v>
       </c>
     </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B117" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A120" s="1" t="s">
         <v>0</v>
@@ -2693,6 +2774,11 @@
         <v>235</v>
       </c>
     </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B127" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A130" s="1" t="s">
         <v>0</v>
@@ -2768,6 +2854,11 @@
         <v>134</v>
       </c>
     </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="B140" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A143" s="1" t="s">
         <v>0</v>
@@ -2798,6 +2889,11 @@
         <v>234</v>
       </c>
     </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="B147" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A150" s="1" t="s">
         <v>0</v>
@@ -2825,6 +2921,11 @@
         <v>208</v>
       </c>
     </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="B154" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A157" s="1" t="s">
         <v>0</v>
@@ -2876,6 +2977,11 @@
         <v>185</v>
       </c>
     </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B164" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A167" s="1" t="s">
         <v>0</v>
@@ -2925,6 +3031,9 @@
       </c>
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B171" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="H171" t="s">
         <v>91</v>
       </c>
@@ -2943,6 +3052,11 @@
         <v>656</v>
       </c>
     </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="H173" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A176" s="1" t="s">
         <v>0</v>
@@ -2960,6 +3074,11 @@
       </c>
       <c r="E178">
         <v>331</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B179" s="1" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.5">
@@ -2989,6 +3108,11 @@
         <v>239</v>
       </c>
     </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B186" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A189" s="1" t="s">
         <v>0</v>
@@ -3008,6 +3132,11 @@
         <v>62</v>
       </c>
     </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B192" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A195" s="1" t="s">
         <v>0</v>
@@ -3025,6 +3154,11 @@
       </c>
       <c r="E197">
         <v>206</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B198" s="1" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.5">
@@ -3054,6 +3188,11 @@
         <v>186</v>
       </c>
     </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B205" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A208" s="1" t="s">
         <v>0</v>
@@ -3081,6 +3220,11 @@
         <v>177</v>
       </c>
     </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B212" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A214" s="1" t="s">
         <v>0</v>
@@ -3108,6 +3252,11 @@
         <v>165</v>
       </c>
     </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B218" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A221" s="1" t="s">
         <v>0</v>
@@ -3159,6 +3308,11 @@
         <v>167</v>
       </c>
     </row>
+    <row r="228" spans="1:43" x14ac:dyDescent="0.5">
+      <c r="B228" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="231" spans="1:43" x14ac:dyDescent="0.5">
       <c r="A231" s="1" t="s">
         <v>0</v>
@@ -3275,6 +3429,9 @@
       <c r="E234">
         <v>237</v>
       </c>
+      <c r="H234" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="N234" t="s">
         <v>118</v>
       </c>
@@ -3286,6 +3443,9 @@
       </c>
       <c r="W234">
         <v>130</v>
+      </c>
+      <c r="AA234" s="1" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="235" spans="1:43" x14ac:dyDescent="0.5">
@@ -3295,6 +3455,19 @@
       <c r="E235">
         <v>110</v>
       </c>
+      <c r="N235" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="T235" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="236" spans="1:43" x14ac:dyDescent="0.5">
+      <c r="B236" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C236" s="1"/>
+      <c r="D236" s="1"/>
     </row>
     <row r="238" spans="1:43" x14ac:dyDescent="0.5">
       <c r="A238" s="1" t="s">
@@ -3315,6 +3488,11 @@
         <v>215</v>
       </c>
     </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B241" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A244" s="1" t="s">
         <v>0</v>
@@ -3332,6 +3510,11 @@
       </c>
       <c r="E246">
         <v>138</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B247" s="1" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.5">
@@ -3369,6 +3552,11 @@
         <v>425</v>
       </c>
     </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B255" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A258" s="1" t="s">
         <v>0</v>
@@ -3396,6 +3584,11 @@
         <v>655</v>
       </c>
     </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B262" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A265" s="1" t="s">
         <v>0</v>
@@ -3423,6 +3616,11 @@
         <v>626</v>
       </c>
     </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B269" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A273" s="1" t="s">
         <v>0</v>
@@ -3442,6 +3640,11 @@
         <v>232</v>
       </c>
     </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B276" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A279" s="1" t="s">
         <v>0</v>
@@ -3459,6 +3662,11 @@
       </c>
       <c r="E281">
         <v>504</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B282" s="1" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.5">
@@ -3496,6 +3704,11 @@
         <v>174</v>
       </c>
     </row>
+    <row r="290" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B290" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="293" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A293" s="1" t="s">
         <v>0</v>
@@ -3513,6 +3726,11 @@
       </c>
       <c r="E295">
         <v>221</v>
+      </c>
+    </row>
+    <row r="296" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B296" s="1" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="300" spans="1:17" x14ac:dyDescent="0.5">
@@ -3577,6 +3795,9 @@
       <c r="K303">
         <v>74</v>
       </c>
+      <c r="N303" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="304" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B304" t="s">
@@ -3593,6 +3814,9 @@
       </c>
     </row>
     <row r="305" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B305" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="H305" t="s">
         <v>32</v>
       </c>
@@ -3640,6 +3864,11 @@
         <v>129</v>
       </c>
     </row>
+    <row r="311" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="H311" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="314" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A314" s="1" t="s">
         <v>0</v>
@@ -3688,6 +3917,14 @@
         <v>118</v>
       </c>
     </row>
+    <row r="318" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B318" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="H318" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="321" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A321" s="1" t="s">
         <v>0</v>
@@ -3707,6 +3944,11 @@
         <v>213</v>
       </c>
     </row>
+    <row r="324" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B324" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="327" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A327" s="1" t="s">
         <v>0</v>
@@ -3756,6 +3998,17 @@
         <v>91</v>
       </c>
     </row>
+    <row r="330" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B330" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="H330" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="N330" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="334" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A334" s="1" t="s">
         <v>0</v>
@@ -3791,6 +4044,9 @@
       </c>
     </row>
     <row r="337" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B337" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="H337" t="s">
         <v>377</v>
       </c>
@@ -3806,6 +4062,11 @@
         <v>134</v>
       </c>
     </row>
+    <row r="339" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="H339" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="340" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A340" s="1" t="s">
         <v>0</v>
@@ -3833,6 +4094,11 @@
         <v>140</v>
       </c>
     </row>
+    <row r="344" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B344" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="347" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A347" s="1" t="s">
         <v>0</v>
@@ -3921,6 +4187,9 @@
       <c r="K351">
         <v>110</v>
       </c>
+      <c r="N351" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="352" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B352" t="s">
@@ -3951,11 +4220,19 @@
       </c>
     </row>
     <row r="354" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B354" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="H354" t="s">
         <v>179</v>
       </c>
       <c r="K354">
         <v>104</v>
+      </c>
+    </row>
+    <row r="355" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="H355" s="1" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="359" spans="1:11" x14ac:dyDescent="0.5">
@@ -4001,6 +4278,11 @@
         <v>130</v>
       </c>
     </row>
+    <row r="365" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B365" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="368" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A368" s="1" t="s">
         <v>0</v>
@@ -4028,6 +4310,11 @@
         <v>114</v>
       </c>
     </row>
+    <row r="372" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B372" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="375" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A375" s="1" t="s">
         <v>0</v>
@@ -4069,6 +4356,9 @@
       <c r="E378">
         <v>113</v>
       </c>
+      <c r="H378" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="379" spans="1:11" x14ac:dyDescent="0.5">
       <c r="B379" t="s">
@@ -4110,6 +4400,11 @@
         <v>120</v>
       </c>
     </row>
+    <row r="384" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B384" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="387" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A387" s="1" t="s">
         <v>0</v>
@@ -4165,6 +4460,9 @@
       <c r="E391">
         <v>107</v>
       </c>
+      <c r="H391" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="392" spans="1:11" x14ac:dyDescent="0.5">
       <c r="B392" t="s">
@@ -4174,6 +4472,11 @@
         <v>143</v>
       </c>
     </row>
+    <row r="393" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B393" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="396" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A396" s="1" t="s">
         <v>0</v>
@@ -4209,6 +4512,11 @@
         <v>230</v>
       </c>
     </row>
+    <row r="401" spans="1:64" x14ac:dyDescent="0.5">
+      <c r="B401" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="404" spans="1:64" x14ac:dyDescent="0.5">
       <c r="A404" s="1" t="s">
         <v>0</v>
@@ -4252,6 +4560,11 @@
         <v>157</v>
       </c>
     </row>
+    <row r="410" spans="1:64" x14ac:dyDescent="0.5">
+      <c r="B410" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="413" spans="1:64" x14ac:dyDescent="0.5">
       <c r="A413" s="1" t="s">
         <v>0</v>
@@ -4402,6 +4715,9 @@
       <c r="H416" t="s">
         <v>198</v>
       </c>
+      <c r="T416" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="AA416" t="s">
         <v>202</v>
       </c>
@@ -4452,6 +4768,12 @@
       <c r="E417">
         <v>149</v>
       </c>
+      <c r="H417" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="N417" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="AA417" s="2" t="s">
         <v>204</v>
       </c>
@@ -4499,6 +4821,9 @@
       <c r="E418">
         <v>94</v>
       </c>
+      <c r="AA418" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="AG418" t="s">
         <v>1</v>
       </c>
@@ -4531,6 +4856,9 @@
       </c>
     </row>
     <row r="419" spans="1:64" x14ac:dyDescent="0.5">
+      <c r="B419" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="AG419" t="s">
         <v>156</v>
       </c>
@@ -4737,6 +5065,23 @@
         <v>383</v>
       </c>
     </row>
+    <row r="431" spans="1:64" x14ac:dyDescent="0.5">
+      <c r="B431" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="H431" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="N431" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="T431" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="AA431" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="435" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A435" s="1" t="s">
         <v>0</v>
@@ -4768,6 +5113,9 @@
       <c r="M437" s="1"/>
     </row>
     <row r="438" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="B438" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="H438" t="s">
         <v>50</v>
       </c>
@@ -4775,6 +5123,11 @@
         <v>93</v>
       </c>
     </row>
+    <row r="439" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="H439" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="441" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A441" s="1" t="s">
         <v>0</v>
@@ -4804,6 +5157,9 @@
       </c>
     </row>
     <row r="444" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="B444" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="H444" t="s">
         <v>241</v>
       </c>
@@ -4842,6 +5198,11 @@
         <v>177</v>
       </c>
     </row>
+    <row r="450" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="H450" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="453" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A453" s="1" t="s">
         <v>0</v>
@@ -4874,6 +5235,9 @@
       </c>
     </row>
     <row r="456" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="B456" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="H456" t="s">
         <v>1</v>
       </c>
@@ -4897,6 +5261,11 @@
         <v>246</v>
       </c>
     </row>
+    <row r="459" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="H459" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="460" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A460" s="1" t="s">
         <v>0</v>
@@ -4938,6 +5307,14 @@
       <c r="E463">
         <v>388</v>
       </c>
+      <c r="H463" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="464" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="B464" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="468" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A468" s="1" t="s">
@@ -4974,6 +5351,9 @@
       <c r="E471">
         <v>203</v>
       </c>
+      <c r="H471" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="472" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B472" t="s">
@@ -5039,6 +5419,11 @@
         <v>171</v>
       </c>
     </row>
+    <row r="480" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B480" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="484" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A484" s="1" t="s">
         <v>0</v>
@@ -5090,6 +5475,11 @@
         <v>198</v>
       </c>
     </row>
+    <row r="491" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B491" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="494" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A494" s="1" t="s">
         <v>0</v>
@@ -5125,6 +5515,9 @@
       </c>
     </row>
     <row r="497" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B497" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="H497" t="s">
         <v>264</v>
       </c>
@@ -5155,6 +5548,11 @@
         <v>268</v>
       </c>
     </row>
+    <row r="502" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="H502" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="505" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A505" s="1" t="s">
         <v>0</v>
@@ -5182,6 +5580,11 @@
         <v>178</v>
       </c>
     </row>
+    <row r="509" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B509" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="512" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A512" s="1" t="s">
         <v>0</v>
@@ -5233,6 +5636,11 @@
         <v>118</v>
       </c>
     </row>
+    <row r="519" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B519" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="522" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A522" s="1" t="s">
         <v>0</v>
@@ -5308,6 +5716,11 @@
         <v>76</v>
       </c>
     </row>
+    <row r="532" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B532" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="535" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A535" s="1" t="s">
         <v>0</v>
@@ -5371,6 +5784,9 @@
       </c>
     </row>
     <row r="540" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B540" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="H540" t="s">
         <v>288</v>
       </c>
@@ -5386,6 +5802,11 @@
         <v>135</v>
       </c>
     </row>
+    <row r="542" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="H542" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="546" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A546" s="1" t="s">
         <v>0</v>
@@ -5426,6 +5847,9 @@
       <c r="E549">
         <v>206</v>
       </c>
+      <c r="H549" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="550" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B550" t="s">
@@ -5443,6 +5867,11 @@
         <v>191</v>
       </c>
     </row>
+    <row r="552" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="B552" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="555" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A555" s="1" t="s">
         <v>0</v>
@@ -5472,6 +5901,11 @@
         <v>231</v>
       </c>
     </row>
+    <row r="559" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="B559" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="563" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A563" s="1" t="s">
         <v>0</v>
@@ -5513,6 +5947,9 @@
       <c r="E566">
         <v>146</v>
       </c>
+      <c r="H566" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="567" spans="1:11" x14ac:dyDescent="0.5">
       <c r="B567" t="s">
@@ -5530,6 +5967,11 @@
         <v>93</v>
       </c>
     </row>
+    <row r="569" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B569" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="572" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A572" s="1" t="s">
         <v>0</v>
@@ -5565,6 +6007,11 @@
         <v>160</v>
       </c>
     </row>
+    <row r="577" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B577" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A580" s="1" t="s">
         <v>0</v>
@@ -5600,6 +6047,11 @@
         <v>160</v>
       </c>
     </row>
+    <row r="585" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B585" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="588" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A588" s="1" t="s">
         <v>0</v>
@@ -5635,6 +6087,11 @@
         <v>160</v>
       </c>
     </row>
+    <row r="593" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B593" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="597" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A597" s="1" t="s">
         <v>0</v>
@@ -5670,6 +6127,11 @@
         <v>158</v>
       </c>
     </row>
+    <row r="602" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B602" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="605" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A605" s="1" t="s">
         <v>0</v>
@@ -5697,6 +6159,11 @@
         <v>249</v>
       </c>
     </row>
+    <row r="609" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B609" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="612" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A612" s="1" t="s">
         <v>0</v>
@@ -5724,6 +6191,11 @@
         <v>151</v>
       </c>
     </row>
+    <row r="616" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B616" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="620" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A620" s="1" t="s">
         <v>0</v>
@@ -5743,6 +6215,11 @@
         <v>455</v>
       </c>
     </row>
+    <row r="623" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B623" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="627" spans="1:28" x14ac:dyDescent="0.5">
       <c r="A627" s="1" t="s">
         <v>0</v>
@@ -5762,6 +6239,11 @@
         <v>384</v>
       </c>
     </row>
+    <row r="630" spans="1:28" x14ac:dyDescent="0.5">
+      <c r="B630" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="633" spans="1:28" x14ac:dyDescent="0.5">
       <c r="A633" s="1" t="s">
         <v>0</v>
@@ -5779,6 +6261,11 @@
       </c>
       <c r="E635">
         <v>352</v>
+      </c>
+    </row>
+    <row r="636" spans="1:28" x14ac:dyDescent="0.5">
+      <c r="B636" s="1" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="639" spans="1:28" x14ac:dyDescent="0.5">
@@ -5867,11 +6354,17 @@
       <c r="E642">
         <v>107</v>
       </c>
+      <c r="H642" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="N642" t="s">
         <v>183</v>
       </c>
       <c r="Q642">
         <v>140</v>
+      </c>
+      <c r="U642" s="1" t="s">
+        <v>385</v>
       </c>
       <c r="AB642" t="s">
         <v>181</v>
@@ -5893,6 +6386,17 @@
       <c r="Q643">
         <v>145</v>
       </c>
+      <c r="AB643" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="644" spans="1:31" x14ac:dyDescent="0.5">
+      <c r="B644" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="N644" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="647" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A647" s="1" t="s">
@@ -5911,6 +6415,11 @@
       </c>
       <c r="E649">
         <v>193</v>
+      </c>
+    </row>
+    <row r="650" spans="1:31" x14ac:dyDescent="0.5">
+      <c r="B650" s="1" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="654" spans="1:31" x14ac:dyDescent="0.5">
@@ -5940,6 +6449,11 @@
         <v>136</v>
       </c>
     </row>
+    <row r="658" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="B658" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="662" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A662" s="1" t="s">
         <v>0</v>
@@ -6008,6 +6522,20 @@
       <c r="E665">
         <v>112</v>
       </c>
+      <c r="H665" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="N665" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="S665" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="666" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="B666" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="670" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A670" s="1" t="s">
@@ -6072,6 +6600,9 @@
       </c>
     </row>
     <row r="675" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B675" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="H675" t="s">
         <v>171</v>
       </c>
@@ -6087,6 +6618,11 @@
         <v>130</v>
       </c>
     </row>
+    <row r="677" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="H677" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="680" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A680" s="1" t="s">
         <v>0</v>
@@ -6128,6 +6664,9 @@
       <c r="E683">
         <v>244</v>
       </c>
+      <c r="H683" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="684" spans="1:11" x14ac:dyDescent="0.5">
       <c r="B684" t="s">
@@ -6145,6 +6684,11 @@
         <v>109</v>
       </c>
     </row>
+    <row r="686" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B686" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="690" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A690" s="1" t="s">
         <v>0</v>
@@ -6177,6 +6721,14 @@
       </c>
       <c r="K692">
         <v>71</v>
+      </c>
+    </row>
+    <row r="693" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B693" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="H693" s="1" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="698" spans="1:11" x14ac:dyDescent="0.5">
@@ -6228,6 +6780,9 @@
       </c>
     </row>
     <row r="702" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B702" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="H702" t="s">
         <v>325</v>
       </c>
@@ -6243,6 +6798,11 @@
         <v>193</v>
       </c>
     </row>
+    <row r="704" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="H704" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="707" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A707" s="1" t="s">
         <v>0</v>
@@ -6286,6 +6846,11 @@
         <v>132</v>
       </c>
     </row>
+    <row r="713" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B713" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="717" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A717" s="1" t="s">
         <v>0</v>
@@ -6353,6 +6918,11 @@
         <v>158</v>
       </c>
     </row>
+    <row r="726" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B726" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="730" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A730" s="1" t="s">
         <v>0</v>
@@ -6412,6 +6982,11 @@
         <v>145</v>
       </c>
     </row>
+    <row r="738" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B738" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="741" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A741" s="1" t="s">
         <v>0</v>
@@ -6465,6 +7040,9 @@
       <c r="E744">
         <v>191</v>
       </c>
+      <c r="H744" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="N744" t="s">
         <v>334</v>
       </c>
@@ -6473,6 +7051,9 @@
       </c>
     </row>
     <row r="745" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="B745" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="N745" t="s">
         <v>335</v>
       </c>
@@ -6488,6 +7069,11 @@
         <v>131</v>
       </c>
     </row>
+    <row r="747" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="N747" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="752" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A752" s="1" t="s">
         <v>0</v>
@@ -6515,6 +7101,11 @@
         <v>279</v>
       </c>
     </row>
+    <row r="756" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B756" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="760" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A760" s="1" t="s">
         <v>0</v>
@@ -6547,6 +7138,14 @@
       </c>
       <c r="K762">
         <v>165</v>
+      </c>
+    </row>
+    <row r="763" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B763" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="H763" s="1" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="768" spans="1:11" x14ac:dyDescent="0.5">
@@ -6577,6 +7176,11 @@
         <v>138</v>
       </c>
     </row>
+    <row r="772" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B772" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="776" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A776" s="1" t="s">
         <v>0</v>
@@ -6604,6 +7208,11 @@
         <v>261</v>
       </c>
     </row>
+    <row r="780" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B780" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="783" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A783" s="1" t="s">
         <v>0</v>
@@ -6623,6 +7232,11 @@
         <v>265</v>
       </c>
     </row>
+    <row r="786" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="B786" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
     <row r="790" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A790" s="1" t="s">
         <v>0</v>
@@ -6667,6 +7281,17 @@
       </c>
       <c r="N792" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="793" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="B793" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="H793" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="N793" s="1" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -6676,6 +7301,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031385706CA3FA84681F867EB376ECE88" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f1fc3953947fc19943d98dadf1eaf13e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="163bd41d-ffc0-4488-8254-6d9532a5df22" xmlns:ns4="fe0a2be5-001b-4af7-88ab-b8670509d488" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eabe67d499736c6c3545e54de71cb0d0" ns3:_="" ns4:_="">
     <xsd:import namespace="163bd41d-ffc0-4488-8254-6d9532a5df22"/>
@@ -6892,22 +7532,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{185A5BC9-AD16-4F95-9710-BE4AF7223593}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCCADD11-3EFF-40DA-B946-3C7FA1B5287A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67C188D1-C88D-41D2-B2A9-E365BBCCA8F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6924,21 +7566,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCCADD11-3EFF-40DA-B946-3C7FA1B5287A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{185A5BC9-AD16-4F95-9710-BE4AF7223593}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Grabbing ItemTypes and Properties then querying for ID data then prior property lengths
</commit_message>
<xml_diff>
--- a/Width Lengths.xlsx
+++ b/Width Lengths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyGit\SQLQueryCreator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469D6E3C-5985-4F89-B237-DB5440DEB5DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F61595-E1E2-4338-8030-41225867C60C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7" yWindow="0" windowWidth="19993" windowHeight="12313" xr2:uid="{BCF4C9D9-7C86-41C2-945B-B1551F976C53}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12920" xr2:uid="{BCF4C9D9-7C86-41C2-945B-B1551F976C53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1609,7 +1609,7 @@
   <dimension ref="A1:BL793"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -7301,21 +7301,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031385706CA3FA84681F867EB376ECE88" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f1fc3953947fc19943d98dadf1eaf13e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="163bd41d-ffc0-4488-8254-6d9532a5df22" xmlns:ns4="fe0a2be5-001b-4af7-88ab-b8670509d488" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eabe67d499736c6c3545e54de71cb0d0" ns3:_="" ns4:_="">
     <xsd:import namespace="163bd41d-ffc0-4488-8254-6d9532a5df22"/>
@@ -7532,24 +7517,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{185A5BC9-AD16-4F95-9710-BE4AF7223593}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCCADD11-3EFF-40DA-B946-3C7FA1B5287A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67C188D1-C88D-41D2-B2A9-E365BBCCA8F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7566,4 +7549,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCCADD11-3EFF-40DA-B946-3C7FA1B5287A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{185A5BC9-AD16-4F95-9710-BE4AF7223593}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Now printing new width length queries to sheet next to property - just need to include something to append next items properly
</commit_message>
<xml_diff>
--- a/Width Lengths.xlsx
+++ b/Width Lengths.xlsx
@@ -438,10 +438,10 @@
   <dimension ref="A1:BL793"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.35" outlineLevelCol="0"/>
   <cols>
     <col width="8.9375" customWidth="1" style="2" min="2" max="2"/>
     <col width="8.9375" customWidth="1" style="2" min="5" max="5"/>
@@ -8355,7 +8355,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8377,6 +8377,26 @@
       <c r="D1" t="n">
         <v>200</v>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>UPDATE innovator.PROPERTY SET COLUMN_WIDTH='250' WHERE NAME='name' AND SOURCE_ID='D4590FC23B0E4E3DBC981F0BFAF4D105'</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>200</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>UPDATE innovator.PROPERTY SET COLUMN_WIDTH='365' WHERE NAME='description' AND SOURCE_ID='D4590FC23B0E4E3DBC981F0BFAF4D105'</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>